<commit_message>
technical data layers updated
</commit_message>
<xml_diff>
--- a/prep_whi/CS_CP_HAB/wetlands/ccap_wetlands_2005.xlsx
+++ b/prep_whi/CS_CP_HAB/wetlands/ccap_wetlands_2005.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="4500" windowWidth="25640" windowHeight="14040" xr2:uid="{4121902A-B0F5-1B4E-A76D-D6C5393DAAEE}"/>
+    <workbookView xWindow="-35520" yWindow="620" windowWidth="25640" windowHeight="14040" xr2:uid="{4121902A-B0F5-1B4E-A76D-D6C5393DAAEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -381,15 +381,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69AA1430-C686-D041-B645-F89466B184AD}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,7 +397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -405,13 +405,27 @@
         <f>52299/1000000</f>
         <v>5.2298999999999998E-2</v>
       </c>
+      <c r="C2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>8.7010000000000004E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="C3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="D3">
+        <f>C3-B3</f>
+        <v>1.5399999999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>